<commit_message>
fixed up programs script, removed unnecesary spreadsheet, changed programs api to use programs table
</commit_message>
<xml_diff>
--- a/spreadsheets/sponsored_2018.xlsx
+++ b/spreadsheets/sponsored_2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5080" windowHeight="8540" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5080" windowHeight="8540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ALL EQUIVALENCIES use Filter " sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11778" uniqueCount="3810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11777" uniqueCount="3810">
   <si>
     <t>ART 5450</t>
   </si>
@@ -12043,7 +12043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1447"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C955" sqref="C955"/>
     </sheetView>
   </sheetViews>
@@ -58975,10 +58975,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A36"/>
+  <dimension ref="A1:A35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -59068,102 +59068,97 @@
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="6" t="s">
-        <v>1304</v>
+      <c r="A17" s="7" t="s">
+        <v>1371</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="7" t="s">
-        <v>1371</v>
+      <c r="A18" s="6" t="s">
+        <v>1397</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="6" t="s">
-        <v>1397</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="6" t="s">
-        <v>1434</v>
+      <c r="A20" s="7" t="s">
+        <v>1821</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="7" t="s">
-        <v>1821</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="7" t="s">
-        <v>1840</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="7" t="s">
-        <v>1853</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="7" t="s">
-        <v>1864</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="7" t="s">
-        <v>1873</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="7" t="s">
-        <v>1879</v>
+      <c r="A26" s="6" t="s">
+        <v>1887</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="6" t="s">
-        <v>1887</v>
+      <c r="A27" s="7" t="s">
+        <v>1899</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="7" t="s">
-        <v>1899</v>
+      <c r="A28" s="6" t="s">
+        <v>1904</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="6" t="s">
-        <v>1904</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="6" t="s">
-        <v>1943</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="6" t="s">
-        <v>2409</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="6" t="s">
-        <v>2471</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="6" t="s">
-        <v>2888</v>
+        <v>3357</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="6" t="s">
-        <v>3357</v>
+        <v>3428</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="6" t="s">
-        <v>3428</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="7" t="s">
+      <c r="A35" s="7" t="s">
         <v>3491</v>
       </c>
     </row>
@@ -60402,7 +60397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added program cities to spreadsheet and db table
</commit_message>
<xml_diff>
--- a/spreadsheets/sponsored_2018.xlsx
+++ b/spreadsheets/sponsored_2018.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11777" uniqueCount="3810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11816" uniqueCount="3849">
   <si>
     <t>ART 5450</t>
   </si>
@@ -11480,17 +11480,141 @@
   <si>
     <t>Writing Enriched Designation</t>
   </si>
+  <si>
+    <t>PROGRAM TYPE</t>
+  </si>
+  <si>
+    <t>HOST URL</t>
+  </si>
+  <si>
+    <t>APPLICATION LINK</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Stellenbosch</t>
+  </si>
+  <si>
+    <t>Akita</t>
+  </si>
+  <si>
+    <t>Copenhagen</t>
+  </si>
+  <si>
+    <t>Oxford</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Cordoba</t>
+  </si>
+  <si>
+    <t>Amman</t>
+  </si>
+  <si>
+    <t>Aix-en-Provence</t>
+  </si>
+  <si>
+    <t>Buenos Aires</t>
+  </si>
+  <si>
+    <t>Valparaiso</t>
+  </si>
+  <si>
+    <t>ISEP Belgium</t>
+  </si>
+  <si>
+    <t>Brussels</t>
+  </si>
+  <si>
+    <t>Graz</t>
+  </si>
+  <si>
+    <t>Legon</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Auckland</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Granada</t>
+  </si>
+  <si>
+    <t>Limerick</t>
+  </si>
+  <si>
+    <t>Washington D.C.</t>
+  </si>
+  <si>
+    <t>Bangkok</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>South Caicos</t>
+  </si>
+  <si>
+    <t>Moyo Hill Camp</t>
+  </si>
+  <si>
+    <t>Cuzco</t>
+  </si>
+  <si>
+    <t>Bocas del Toro</t>
+  </si>
+  <si>
+    <t>Atherton Tablelands</t>
+  </si>
+  <si>
+    <t>Siem Reap</t>
+  </si>
+  <si>
+    <t>Atenas</t>
+  </si>
+  <si>
+    <t>Bumthang</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Lato"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -11652,114 +11776,116 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12043,8 +12169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1447"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C955" sqref="C955"/>
+    <sheetView topLeftCell="A519" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A533" sqref="A533"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -58975,10 +59101,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -58987,183 +59113,308 @@
     <col min="2" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>3589</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="65" t="s">
+        <v>3810</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>3811</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>3812</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>3813</v>
+      </c>
+      <c r="F1" s="65" t="s">
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
         <v>3543</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="E2" s="65" t="s">
+        <v>3815</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="E3" s="65" t="s">
+        <v>3820</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="E4" s="65" t="s">
+        <v>3816</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="E5" s="65" t="s">
+        <v>3817</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="E6" s="65" t="s">
+        <v>3824</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="7" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="E7" s="65" t="s">
+        <v>3825</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="7" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="E8" s="65" t="s">
+        <v>3823</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="E9" s="65" t="s">
+        <v>3818</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="E10" s="65" t="s">
+        <v>3826</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="6" t="s">
         <v>921</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="E11" s="65" t="s">
+        <v>3827</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="6" t="s">
         <v>971</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="6" t="s">
-        <v>3542</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="E12" s="65" t="s">
+        <v>3828</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="66" t="s">
+        <v>3829</v>
+      </c>
+      <c r="E13" s="65" t="s">
+        <v>3830</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="6" t="s">
         <v>1159</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="E14" s="65" t="s">
+        <v>3831</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="6" t="s">
         <v>1228</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="E15" s="65" t="s">
+        <v>3832</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="6" t="s">
         <v>1290</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="E16" s="65" t="s">
+        <v>3839</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="7" t="s">
         <v>1371</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="E17" s="65" t="s">
+        <v>3821</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="6" t="s">
         <v>1397</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="E18" s="65" t="s">
+        <v>3819</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="6" t="s">
         <v>1434</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="E19" s="65" t="s">
+        <v>3815</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="7" t="s">
         <v>1821</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="E20" s="65" t="s">
+        <v>3845</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="7" t="s">
         <v>1840</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="E21" s="65" t="s">
+        <v>3848</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
         <v>1853</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="E22" s="65" t="s">
+        <v>3846</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="7" t="s">
         <v>1864</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="E23" s="65" t="s">
+        <v>3847</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="7" t="s">
         <v>1873</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="E24" s="65" t="s">
+        <v>3844</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="7" t="s">
         <v>1879</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="E25" s="65" t="s">
+        <v>3843</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="6" t="s">
         <v>1887</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="E26" s="65" t="s">
+        <v>3842</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="7" t="s">
         <v>1899</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="E27" s="65" t="s">
+        <v>3841</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="6" t="s">
         <v>1904</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="E28" s="65" t="s">
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="6" t="s">
         <v>1943</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="E29" s="65" t="s">
+        <v>3833</v>
+      </c>
+      <c r="F29" s="65"/>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="6" t="s">
         <v>2409</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="E30" s="65" t="s">
+        <v>3822</v>
+      </c>
+      <c r="F30" s="65"/>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="6" t="s">
         <v>2471</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="E31" s="65" t="s">
+        <v>3834</v>
+      </c>
+      <c r="F31" s="65"/>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="6" t="s">
         <v>2888</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="E32" s="65" t="s">
+        <v>3835</v>
+      </c>
+      <c r="F32" s="65"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="6" t="s">
         <v>3357</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="E33" s="65" t="s">
+        <v>3836</v>
+      </c>
+      <c r="F33" s="65"/>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="6" t="s">
         <v>3428</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="E34" s="65" t="s">
+        <v>3837</v>
+      </c>
+      <c r="F34" s="65"/>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="7" t="s">
         <v>3491</v>
       </c>
+      <c r="E35" s="65" t="s">
+        <v>3838</v>
+      </c>
+      <c r="F35" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added country for all programs
</commit_message>
<xml_diff>
--- a/spreadsheets/sponsored_2018.xlsx
+++ b/spreadsheets/sponsored_2018.xlsx
@@ -11493,118 +11493,125 @@
     <t>COUNTRY</t>
   </si>
   <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t>Stellenbosch</t>
-  </si>
-  <si>
-    <t>Akita</t>
-  </si>
-  <si>
-    <t>Copenhagen</t>
-  </si>
-  <si>
-    <t>Paris</t>
-  </si>
-  <si>
-    <t>Rome</t>
-  </si>
-  <si>
-    <t>Beijing</t>
-  </si>
-  <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>Cordoba</t>
-  </si>
-  <si>
-    <t>Amman</t>
-  </si>
-  <si>
-    <t>Aix-en-Provence</t>
-  </si>
-  <si>
-    <t>Buenos Aires</t>
-  </si>
-  <si>
-    <t>Valparaiso</t>
-  </si>
-  <si>
     <t>ISEP Belgium</t>
   </si>
   <si>
-    <t>Brussels</t>
-  </si>
-  <si>
-    <t>Graz</t>
-  </si>
-  <si>
-    <t>Legon</t>
-  </si>
-  <si>
-    <t>Madrid</t>
-  </si>
-  <si>
-    <t>Auckland</t>
-  </si>
-  <si>
-    <t>Glasgow</t>
-  </si>
-  <si>
-    <t>Granada</t>
-  </si>
-  <si>
-    <t>Limerick</t>
-  </si>
-  <si>
-    <t>Washington D.C.</t>
-  </si>
-  <si>
-    <t>Bangkok</t>
-  </si>
-  <si>
-    <t>Tokyo</t>
-  </si>
-  <si>
-    <t>South Caicos</t>
-  </si>
-  <si>
-    <t>Moyo Hill Camp</t>
-  </si>
-  <si>
-    <t>Cuzco</t>
-  </si>
-  <si>
-    <t>Bocas del Toro</t>
-  </si>
-  <si>
-    <t>Atherton Tablelands</t>
-  </si>
-  <si>
-    <t>Siem Reap</t>
-  </si>
-  <si>
-    <t>Atenas</t>
-  </si>
-  <si>
-    <t>Bumthang</t>
-  </si>
-  <si>
     <t>Oxford, England</t>
+  </si>
+  <si>
+    <t>London, England</t>
+  </si>
+  <si>
+    <t>Paris, France</t>
+  </si>
+  <si>
+    <t>Stellenbosch, South Africa</t>
+  </si>
+  <si>
+    <t>Akita, Japan</t>
+  </si>
+  <si>
+    <t>Cordoba, Argentina</t>
+  </si>
+  <si>
+    <t>Amman, Jordan</t>
+  </si>
+  <si>
+    <t>Hyderabad, India</t>
+  </si>
+  <si>
+    <t>Copenhagen, Denmark</t>
+  </si>
+  <si>
+    <t>Aix-en-Provence, France</t>
+  </si>
+  <si>
+    <t>Buenos Aires, Argentina</t>
+  </si>
+  <si>
+    <t>Valparaiso, Chile</t>
+  </si>
+  <si>
+    <t>Brussels, Belgium</t>
+  </si>
+  <si>
+    <t>Graz, Austria</t>
+  </si>
+  <si>
+    <t>Legon, Ghana</t>
+  </si>
+  <si>
+    <t>Bangkok, Thailand</t>
+  </si>
+  <si>
+    <t>Rome, Italy</t>
+  </si>
+  <si>
+    <t>Atherton Tablelands, Australia</t>
+  </si>
+  <si>
+    <t>Bumthang, Bhutan</t>
+  </si>
+  <si>
+    <t>Siem Reap, Cambodia</t>
+  </si>
+  <si>
+    <t>Atenas, Costa Rica</t>
+  </si>
+  <si>
+    <t>Bocas del Toro, Panama</t>
+  </si>
+  <si>
+    <t>Cuzco, Peru</t>
+  </si>
+  <si>
+    <t>Moyo Hill Camp, Tanzania</t>
+  </si>
+  <si>
+    <t>South Caicos, Turks and Caicos</t>
+  </si>
+  <si>
+    <t>Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Madrid, Spain</t>
+  </si>
+  <si>
+    <t>Beijing, China</t>
+  </si>
+  <si>
+    <t>Auckland, New Zealand</t>
+  </si>
+  <si>
+    <t>Glasgow, Scotland</t>
+  </si>
+  <si>
+    <t>Granada, Spain</t>
+  </si>
+  <si>
+    <t>Limerick, Ireland</t>
+  </si>
+  <si>
+    <t>Washington D.C., USA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Lato"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -11780,116 +11787,117 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -27058,7 +27066,7 @@
     </row>
     <row r="461" spans="1:12" ht="15.5">
       <c r="A461" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B461" s="8" t="s">
         <v>1307</v>
@@ -27094,7 +27102,7 @@
     </row>
     <row r="462" spans="1:12" ht="15.5">
       <c r="A462" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B462" s="8" t="s">
         <v>1309</v>
@@ -27126,7 +27134,7 @@
     </row>
     <row r="463" spans="1:12" ht="15.5">
       <c r="A463" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B463" s="8" t="s">
         <v>1310</v>
@@ -27158,7 +27166,7 @@
     </row>
     <row r="464" spans="1:12" ht="15.5">
       <c r="A464" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B464" s="9" t="s">
         <v>1313</v>
@@ -27190,7 +27198,7 @@
     </row>
     <row r="465" spans="1:12" ht="15.5">
       <c r="A465" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B465" s="8" t="s">
         <v>1317</v>
@@ -27224,7 +27232,7 @@
     </row>
     <row r="466" spans="1:12" ht="15.5">
       <c r="A466" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B466" s="8" t="s">
         <v>1320</v>
@@ -27256,7 +27264,7 @@
     </row>
     <row r="467" spans="1:12" ht="15.5">
       <c r="A467" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B467" s="8" t="s">
         <v>1324</v>
@@ -27290,7 +27298,7 @@
     </row>
     <row r="468" spans="1:12" ht="15.5">
       <c r="A468" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B468" s="8" t="s">
         <v>1326</v>
@@ -27322,7 +27330,7 @@
     </row>
     <row r="469" spans="1:12" ht="15.5">
       <c r="A469" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B469" s="8" t="s">
         <v>1328</v>
@@ -27354,7 +27362,7 @@
     </row>
     <row r="470" spans="1:12" ht="15.5">
       <c r="A470" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B470" s="8" t="s">
         <v>1332</v>
@@ -27388,7 +27396,7 @@
     </row>
     <row r="471" spans="1:12" ht="15.5">
       <c r="A471" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B471" s="37" t="s">
         <v>1334</v>
@@ -27420,7 +27428,7 @@
     </row>
     <row r="472" spans="1:12" ht="15.5">
       <c r="A472" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B472" s="8" t="s">
         <v>1337</v>
@@ -27454,7 +27462,7 @@
     </row>
     <row r="473" spans="1:12" ht="15.5">
       <c r="A473" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B473" s="8" t="s">
         <v>1341</v>
@@ -27488,7 +27496,7 @@
     </row>
     <row r="474" spans="1:12" ht="15.5">
       <c r="A474" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B474" s="8" t="s">
         <v>3574</v>
@@ -27522,7 +27530,7 @@
     </row>
     <row r="475" spans="1:12" ht="15.5">
       <c r="A475" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B475" s="8" t="s">
         <v>1343</v>
@@ -27556,7 +27564,7 @@
     </row>
     <row r="476" spans="1:12" ht="15.5">
       <c r="A476" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B476" s="8" t="s">
         <v>1346</v>
@@ -27590,7 +27598,7 @@
     </row>
     <row r="477" spans="1:12" ht="15.5">
       <c r="A477" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B477" s="8" t="s">
         <v>1349</v>
@@ -27624,7 +27632,7 @@
     </row>
     <row r="478" spans="1:12" ht="15.5">
       <c r="A478" s="8" t="s">
-        <v>3827</v>
+        <v>3814</v>
       </c>
       <c r="B478" s="15"/>
       <c r="C478" s="8" t="s">
@@ -59108,14 +59116,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26.58203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="3"/>
+    <col min="2" max="4" width="9" style="3"/>
+    <col min="5" max="5" width="21.9140625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -59142,71 +59152,71 @@
       <c r="A2" s="6" t="s">
         <v>3542</v>
       </c>
-      <c r="E2" s="65" t="s">
-        <v>3814</v>
+      <c r="E2" s="68" t="s">
+        <v>3816</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="65" t="s">
-        <v>3818</v>
+      <c r="E3" s="68" t="s">
+        <v>3817</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="65" t="s">
-        <v>3815</v>
+      <c r="E4" s="68" t="s">
+        <v>3818</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="E5" s="65" t="s">
-        <v>3816</v>
+      <c r="E5" s="68" t="s">
+        <v>3819</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="E6" s="65" t="s">
-        <v>3822</v>
+      <c r="E6" s="68" t="s">
+        <v>3820</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="7" t="s">
         <v>493</v>
       </c>
-      <c r="E7" s="65" t="s">
-        <v>3823</v>
+      <c r="E7" s="68" t="s">
+        <v>3821</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="E8" s="65" t="s">
-        <v>3821</v>
+      <c r="E8" s="68" t="s">
+        <v>3822</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
         <v>598</v>
       </c>
-      <c r="E9" s="65" t="s">
-        <v>3817</v>
+      <c r="E9" s="68" t="s">
+        <v>3823</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
         <v>751</v>
       </c>
-      <c r="E10" s="65" t="s">
+      <c r="E10" s="68" t="s">
         <v>3824</v>
       </c>
     </row>
@@ -59214,7 +59224,7 @@
       <c r="A11" s="6" t="s">
         <v>921</v>
       </c>
-      <c r="E11" s="65" t="s">
+      <c r="E11" s="68" t="s">
         <v>3825</v>
       </c>
     </row>
@@ -59222,48 +59232,48 @@
       <c r="A12" s="6" t="s">
         <v>971</v>
       </c>
-      <c r="E12" s="65" t="s">
+      <c r="E12" s="68" t="s">
         <v>3826</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="66" t="s">
+        <v>3814</v>
+      </c>
+      <c r="E13" s="68" t="s">
         <v>3827</v>
-      </c>
-      <c r="E13" s="65" t="s">
-        <v>3828</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="6" t="s">
         <v>1159</v>
       </c>
-      <c r="E14" s="65" t="s">
-        <v>3829</v>
+      <c r="E14" s="68" t="s">
+        <v>3828</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="6" t="s">
         <v>1228</v>
       </c>
-      <c r="E15" s="65" t="s">
-        <v>3830</v>
+      <c r="E15" s="68" t="s">
+        <v>3829</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="6" t="s">
         <v>1290</v>
       </c>
-      <c r="E16" s="65" t="s">
-        <v>3837</v>
+      <c r="E16" s="68" t="s">
+        <v>3830</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="7" t="s">
         <v>1371</v>
       </c>
-      <c r="E17" s="65" t="s">
-        <v>3819</v>
+      <c r="E17" s="68" t="s">
+        <v>3831</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -59271,78 +59281,78 @@
         <v>1397</v>
       </c>
       <c r="E18" s="67" t="s">
-        <v>3847</v>
+        <v>3815</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="6" t="s">
         <v>1434</v>
       </c>
-      <c r="E19" s="65" t="s">
-        <v>3814</v>
+      <c r="E19" s="68" t="s">
+        <v>3816</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="7" t="s">
         <v>1821</v>
       </c>
-      <c r="E20" s="65" t="s">
-        <v>3843</v>
+      <c r="E20" s="68" t="s">
+        <v>3832</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="7" t="s">
         <v>1840</v>
       </c>
-      <c r="E21" s="65" t="s">
-        <v>3846</v>
+      <c r="E21" s="68" t="s">
+        <v>3833</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
         <v>1853</v>
       </c>
-      <c r="E22" s="65" t="s">
-        <v>3844</v>
+      <c r="E22" s="68" t="s">
+        <v>3834</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="7" t="s">
         <v>1864</v>
       </c>
-      <c r="E23" s="65" t="s">
-        <v>3845</v>
+      <c r="E23" s="68" t="s">
+        <v>3835</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="7" t="s">
         <v>1873</v>
       </c>
-      <c r="E24" s="65" t="s">
-        <v>3842</v>
+      <c r="E24" s="68" t="s">
+        <v>3836</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="7" t="s">
         <v>1879</v>
       </c>
-      <c r="E25" s="65" t="s">
-        <v>3841</v>
+      <c r="E25" s="68" t="s">
+        <v>3837</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="6" t="s">
         <v>1887</v>
       </c>
-      <c r="E26" s="65" t="s">
-        <v>3840</v>
+      <c r="E26" s="68" t="s">
+        <v>3838</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="7" t="s">
         <v>1899</v>
       </c>
-      <c r="E27" s="65" t="s">
+      <c r="E27" s="68" t="s">
         <v>3839</v>
       </c>
     </row>
@@ -59350,16 +59360,16 @@
       <c r="A28" s="6" t="s">
         <v>1904</v>
       </c>
-      <c r="E28" s="65" t="s">
-        <v>3838</v>
+      <c r="E28" s="68" t="s">
+        <v>3840</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="6" t="s">
         <v>1943</v>
       </c>
-      <c r="E29" s="65" t="s">
-        <v>3831</v>
+      <c r="E29" s="68" t="s">
+        <v>3841</v>
       </c>
       <c r="F29" s="65"/>
     </row>
@@ -59367,8 +59377,8 @@
       <c r="A30" s="6" t="s">
         <v>2409</v>
       </c>
-      <c r="E30" s="65" t="s">
-        <v>3820</v>
+      <c r="E30" s="68" t="s">
+        <v>3842</v>
       </c>
       <c r="F30" s="65"/>
     </row>
@@ -59376,8 +59386,8 @@
       <c r="A31" s="6" t="s">
         <v>2471</v>
       </c>
-      <c r="E31" s="65" t="s">
-        <v>3832</v>
+      <c r="E31" s="68" t="s">
+        <v>3843</v>
       </c>
       <c r="F31" s="65"/>
     </row>
@@ -59385,8 +59395,8 @@
       <c r="A32" s="6" t="s">
         <v>2888</v>
       </c>
-      <c r="E32" s="65" t="s">
-        <v>3833</v>
+      <c r="E32" s="68" t="s">
+        <v>3844</v>
       </c>
       <c r="F32" s="65"/>
     </row>
@@ -59394,8 +59404,8 @@
       <c r="A33" s="6" t="s">
         <v>3357</v>
       </c>
-      <c r="E33" s="65" t="s">
-        <v>3834</v>
+      <c r="E33" s="68" t="s">
+        <v>3845</v>
       </c>
       <c r="F33" s="65"/>
     </row>
@@ -59403,8 +59413,8 @@
       <c r="A34" s="6" t="s">
         <v>3428</v>
       </c>
-      <c r="E34" s="65" t="s">
-        <v>3835</v>
+      <c r="E34" s="68" t="s">
+        <v>3846</v>
       </c>
       <c r="F34" s="65"/>
     </row>
@@ -59412,8 +59422,8 @@
       <c r="A35" s="7" t="s">
         <v>3491</v>
       </c>
-      <c r="E35" s="65" t="s">
-        <v>3836</v>
+      <c r="E35" s="68" t="s">
+        <v>3847</v>
       </c>
       <c r="F35" s="65"/>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet and script to include lat/lng
</commit_message>
<xml_diff>
--- a/spreadsheets/sponsored_2018.xlsx
+++ b/spreadsheets/sponsored_2018.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11816" uniqueCount="3848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11817" uniqueCount="3849">
   <si>
     <t>ART 5450</t>
   </si>
@@ -11490,9 +11490,6 @@
     <t>CITY</t>
   </si>
   <si>
-    <t>COUNTRY</t>
-  </si>
-  <si>
     <t>ISEP Belgium</t>
   </si>
   <si>
@@ -11593,18 +11590,31 @@
   </si>
   <si>
     <t>Washington D.C., USA</t>
+  </si>
+  <si>
+    <t>LATITUDE</t>
+  </si>
+  <si>
+    <t>LONGITUDE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Lato"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -11787,116 +11797,117 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -27066,7 +27077,7 @@
     </row>
     <row r="461" spans="1:12" ht="15.5">
       <c r="A461" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B461" s="8" t="s">
         <v>1307</v>
@@ -27102,7 +27113,7 @@
     </row>
     <row r="462" spans="1:12" ht="15.5">
       <c r="A462" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B462" s="8" t="s">
         <v>1309</v>
@@ -27134,7 +27145,7 @@
     </row>
     <row r="463" spans="1:12" ht="15.5">
       <c r="A463" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B463" s="8" t="s">
         <v>1310</v>
@@ -27166,7 +27177,7 @@
     </row>
     <row r="464" spans="1:12" ht="15.5">
       <c r="A464" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B464" s="9" t="s">
         <v>1313</v>
@@ -27198,7 +27209,7 @@
     </row>
     <row r="465" spans="1:12" ht="15.5">
       <c r="A465" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B465" s="8" t="s">
         <v>1317</v>
@@ -27232,7 +27243,7 @@
     </row>
     <row r="466" spans="1:12" ht="15.5">
       <c r="A466" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B466" s="8" t="s">
         <v>1320</v>
@@ -27264,7 +27275,7 @@
     </row>
     <row r="467" spans="1:12" ht="15.5">
       <c r="A467" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B467" s="8" t="s">
         <v>1324</v>
@@ -27298,7 +27309,7 @@
     </row>
     <row r="468" spans="1:12" ht="15.5">
       <c r="A468" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B468" s="8" t="s">
         <v>1326</v>
@@ -27330,7 +27341,7 @@
     </row>
     <row r="469" spans="1:12" ht="15.5">
       <c r="A469" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B469" s="8" t="s">
         <v>1328</v>
@@ -27362,7 +27373,7 @@
     </row>
     <row r="470" spans="1:12" ht="15.5">
       <c r="A470" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B470" s="8" t="s">
         <v>1332</v>
@@ -27396,7 +27407,7 @@
     </row>
     <row r="471" spans="1:12" ht="15.5">
       <c r="A471" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B471" s="37" t="s">
         <v>1334</v>
@@ -27428,7 +27439,7 @@
     </row>
     <row r="472" spans="1:12" ht="15.5">
       <c r="A472" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B472" s="8" t="s">
         <v>1337</v>
@@ -27462,7 +27473,7 @@
     </row>
     <row r="473" spans="1:12" ht="15.5">
       <c r="A473" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B473" s="8" t="s">
         <v>1341</v>
@@ -27496,7 +27507,7 @@
     </row>
     <row r="474" spans="1:12" ht="15.5">
       <c r="A474" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B474" s="8" t="s">
         <v>3574</v>
@@ -27530,7 +27541,7 @@
     </row>
     <row r="475" spans="1:12" ht="15.5">
       <c r="A475" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B475" s="8" t="s">
         <v>1343</v>
@@ -27564,7 +27575,7 @@
     </row>
     <row r="476" spans="1:12" ht="15.5">
       <c r="A476" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B476" s="8" t="s">
         <v>1346</v>
@@ -27598,7 +27609,7 @@
     </row>
     <row r="477" spans="1:12" ht="15.5">
       <c r="A477" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B477" s="8" t="s">
         <v>1349</v>
@@ -27632,7 +27643,7 @@
     </row>
     <row r="478" spans="1:12" ht="15.5">
       <c r="A478" s="8" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B478" s="15"/>
       <c r="C478" s="8" t="s">
@@ -59114,10 +59125,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -59125,10 +59136,12 @@
     <col min="1" max="1" width="26.58203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="9" style="3"/>
     <col min="5" max="5" width="21.9140625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="3"/>
+    <col min="6" max="6" width="15.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>3588</v>
       </c>
@@ -59144,288 +59157,488 @@
       <c r="E1" s="65" t="s">
         <v>3812</v>
       </c>
-      <c r="F1" s="65" t="s">
-        <v>3813</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="F1" s="69" t="s">
+        <v>3847</v>
+      </c>
+      <c r="G1" s="69" t="s">
+        <v>3848</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
         <v>3542</v>
       </c>
       <c r="E2" s="68" t="s">
-        <v>3816</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>3815</v>
+      </c>
+      <c r="F2" s="3">
+        <v>51.507350899999999</v>
+      </c>
+      <c r="G2" s="3">
+        <v>-0.12775829999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
         <v>72</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>3817</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>3816</v>
+      </c>
+      <c r="F3" s="3">
+        <v>48.856614</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2.3522219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="6" t="s">
         <v>128</v>
       </c>
       <c r="E4" s="68" t="s">
-        <v>3818</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>3817</v>
+      </c>
+      <c r="F4" s="3">
+        <v>-33.932104500000001</v>
+      </c>
+      <c r="G4" s="3">
+        <v>18.860151999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
         <v>289</v>
       </c>
       <c r="E5" s="68" t="s">
-        <v>3819</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>3818</v>
+      </c>
+      <c r="F5" s="3">
+        <v>39.718613499999996</v>
+      </c>
+      <c r="G5" s="3">
+        <v>140.1023643</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
         <v>478</v>
       </c>
       <c r="E6" s="68" t="s">
-        <v>3820</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>3819</v>
+      </c>
+      <c r="F6" s="3">
+        <v>31.420083299999899</v>
+      </c>
+      <c r="G6" s="3">
+        <v>-64.188776099999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="7" t="s">
         <v>493</v>
       </c>
       <c r="E7" s="68" t="s">
-        <v>3821</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>3820</v>
+      </c>
+      <c r="F7" s="3">
+        <v>31.9453666</v>
+      </c>
+      <c r="G7" s="3">
+        <v>35.928371599999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
         <v>558</v>
       </c>
       <c r="E8" s="68" t="s">
-        <v>3822</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>3821</v>
+      </c>
+      <c r="F8" s="3">
+        <v>17.385044000000001</v>
+      </c>
+      <c r="G8" s="3">
+        <v>78.486671000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="6" t="s">
         <v>598</v>
       </c>
       <c r="E9" s="68" t="s">
-        <v>3823</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>3822</v>
+      </c>
+      <c r="F9" s="3">
+        <v>55.676096800000003</v>
+      </c>
+      <c r="G9" s="3">
+        <v>12.5683372</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
         <v>751</v>
       </c>
       <c r="E10" s="68" t="s">
-        <v>3824</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>3823</v>
+      </c>
+      <c r="F10" s="3">
+        <v>43.529741999999999</v>
+      </c>
+      <c r="G10" s="3">
+        <v>5.4474269999999896</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="6" t="s">
         <v>921</v>
       </c>
       <c r="E11" s="68" t="s">
-        <v>3825</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>3824</v>
+      </c>
+      <c r="F11" s="3">
+        <v>34.603684399999999</v>
+      </c>
+      <c r="G11" s="3">
+        <v>-58.381559099999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
         <v>971</v>
       </c>
       <c r="E12" s="68" t="s">
+        <v>3825</v>
+      </c>
+      <c r="F12" s="3">
+        <v>-33.047238</v>
+      </c>
+      <c r="G12" s="3">
+        <v>71.612688499999905</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="66" t="s">
+        <v>3813</v>
+      </c>
+      <c r="E13" s="68" t="s">
         <v>3826</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="66" t="s">
-        <v>3814</v>
-      </c>
-      <c r="E13" s="68" t="s">
-        <v>3827</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="F13" s="3">
+        <v>50.850346299999998</v>
+      </c>
+      <c r="G13" s="3">
+        <v>4.3517210999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="6" t="s">
         <v>1159</v>
       </c>
       <c r="E14" s="68" t="s">
-        <v>3828</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>3827</v>
+      </c>
+      <c r="F14" s="3">
+        <v>47.070714000000002</v>
+      </c>
+      <c r="G14" s="3">
+        <v>15.439503999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="6" t="s">
         <v>1228</v>
       </c>
       <c r="E15" s="68" t="s">
-        <v>3829</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>3828</v>
+      </c>
+      <c r="F15" s="3">
+        <v>5.6358281000000003</v>
+      </c>
+      <c r="G15" s="3">
+        <v>-0.16135920000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="6" t="s">
         <v>1290</v>
       </c>
       <c r="E16" s="68" t="s">
-        <v>3830</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>3829</v>
+      </c>
+      <c r="F16" s="3">
+        <v>13.7563309</v>
+      </c>
+      <c r="G16" s="3">
+        <v>100.5017651</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="7" t="s">
         <v>1371</v>
       </c>
       <c r="E17" s="68" t="s">
-        <v>3831</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>3830</v>
+      </c>
+      <c r="F17" s="3">
+        <v>41.902783499999998</v>
+      </c>
+      <c r="G17" s="3">
+        <v>12.4963655</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
         <v>1397</v>
       </c>
       <c r="E18" s="67" t="s">
-        <v>3815</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>3814</v>
+      </c>
+      <c r="F18" s="3">
+        <v>51.752020899999998</v>
+      </c>
+      <c r="G18" s="3">
+        <v>-1.2577263000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
         <v>1434</v>
       </c>
       <c r="E19" s="68" t="s">
-        <v>3816</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>3815</v>
+      </c>
+      <c r="F19" s="3">
+        <v>51.507350899999999</v>
+      </c>
+      <c r="G19" s="3">
+        <v>-0.12775829999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="7" t="s">
         <v>1821</v>
       </c>
       <c r="E20" s="68" t="s">
-        <v>3832</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>3831</v>
+      </c>
+      <c r="F20" s="3">
+        <v>-17.2660801</v>
+      </c>
+      <c r="G20" s="3">
+        <v>145.48585990000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="7" t="s">
         <v>1840</v>
       </c>
       <c r="E21" s="68" t="s">
-        <v>3833</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>3832</v>
+      </c>
+      <c r="F21" s="3">
+        <v>27.641839000000001</v>
+      </c>
+      <c r="G21" s="3">
+        <v>90.677304599999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="7" t="s">
         <v>1853</v>
       </c>
       <c r="E22" s="68" t="s">
-        <v>3834</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>3833</v>
+      </c>
+      <c r="F22" s="3">
+        <v>13.3550091</v>
+      </c>
+      <c r="G22" s="3">
+        <v>103.85517299999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="7" t="s">
         <v>1864</v>
       </c>
       <c r="E23" s="68" t="s">
-        <v>3835</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>3834</v>
+      </c>
+      <c r="F23" s="3">
+        <v>9.9784936000000002</v>
+      </c>
+      <c r="G23" s="3">
+        <v>-84.373839399999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="7" t="s">
         <v>1873</v>
       </c>
       <c r="E24" s="68" t="s">
-        <v>3836</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>3835</v>
+      </c>
+      <c r="F24" s="3">
+        <v>9.4165520999999899</v>
+      </c>
+      <c r="G24" s="3">
+        <v>-82.520778699999994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="7" t="s">
         <v>1879</v>
       </c>
       <c r="E25" s="68" t="s">
-        <v>3837</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>3836</v>
+      </c>
+      <c r="F25" s="3">
+        <v>-13.53195</v>
+      </c>
+      <c r="G25" s="3">
+        <v>-71.967462599999905</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="6" t="s">
         <v>1887</v>
       </c>
       <c r="E26" s="68" t="s">
-        <v>3838</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>3837</v>
+      </c>
+      <c r="F26" s="3">
+        <v>3.3175192999999998</v>
+      </c>
+      <c r="G26" s="3">
+        <v>35.734195300000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="7" t="s">
         <v>1899</v>
       </c>
       <c r="E27" s="68" t="s">
-        <v>3839</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>3838</v>
+      </c>
+      <c r="F27" s="3">
+        <v>21.511236499999999</v>
+      </c>
+      <c r="G27" s="3">
+        <v>-71.518979999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="6" t="s">
         <v>1904</v>
       </c>
       <c r="E28" s="68" t="s">
-        <v>3840</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>3839</v>
+      </c>
+      <c r="F28" s="3">
+        <v>35.689487499999998</v>
+      </c>
+      <c r="G28" s="3">
+        <v>139.69170639999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="6" t="s">
         <v>1943</v>
       </c>
       <c r="E29" s="68" t="s">
-        <v>3841</v>
-      </c>
-      <c r="F29" s="65"/>
-    </row>
-    <row r="30" spans="1:6">
+        <v>3840</v>
+      </c>
+      <c r="F29" s="65">
+        <v>40.416775399999999</v>
+      </c>
+      <c r="G29" s="3">
+        <v>-3.7037901999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="6" t="s">
         <v>2409</v>
       </c>
       <c r="E30" s="68" t="s">
-        <v>3842</v>
-      </c>
-      <c r="F30" s="65"/>
-    </row>
-    <row r="31" spans="1:6">
+        <v>3841</v>
+      </c>
+      <c r="F30" s="65">
+        <v>39.904199899999902</v>
+      </c>
+      <c r="G30" s="3">
+        <v>116.4073963</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="6" t="s">
         <v>2471</v>
       </c>
       <c r="E31" s="68" t="s">
-        <v>3843</v>
-      </c>
-      <c r="F31" s="65"/>
-    </row>
-    <row r="32" spans="1:6">
+        <v>3842</v>
+      </c>
+      <c r="F31" s="65">
+        <v>-36.848459699999999</v>
+      </c>
+      <c r="G31" s="3">
+        <v>174.76333149999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="6" t="s">
         <v>2888</v>
       </c>
       <c r="E32" s="68" t="s">
-        <v>3844</v>
-      </c>
-      <c r="F32" s="65"/>
-    </row>
-    <row r="33" spans="1:6">
+        <v>3843</v>
+      </c>
+      <c r="F32" s="65">
+        <v>55.864237000000003</v>
+      </c>
+      <c r="G32" s="3">
+        <v>-4.2518060000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="6" t="s">
         <v>3357</v>
       </c>
       <c r="E33" s="68" t="s">
-        <v>3845</v>
-      </c>
-      <c r="F33" s="65"/>
-    </row>
-    <row r="34" spans="1:6">
+        <v>3844</v>
+      </c>
+      <c r="F33" s="65">
+        <v>37.1773363</v>
+      </c>
+      <c r="G33" s="3">
+        <v>-3.5985570999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="6" t="s">
         <v>3428</v>
       </c>
       <c r="E34" s="68" t="s">
-        <v>3846</v>
-      </c>
-      <c r="F34" s="65"/>
-    </row>
-    <row r="35" spans="1:6">
+        <v>3845</v>
+      </c>
+      <c r="F34" s="65">
+        <v>52.663836699999997</v>
+      </c>
+      <c r="G34" s="3">
+        <v>-8.6267343000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="7" t="s">
         <v>3491</v>
       </c>
       <c r="E35" s="68" t="s">
-        <v>3847</v>
-      </c>
-      <c r="F35" s="65"/>
+        <v>3846</v>
+      </c>
+      <c r="F35" s="65">
+        <v>38.907192299999998</v>
+      </c>
+      <c r="G35" s="3">
+        <v>-77.036870699999994</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
missed some negatives in the lat/long
</commit_message>
<xml_diff>
--- a/spreadsheets/sponsored_2018.xlsx
+++ b/spreadsheets/sponsored_2018.xlsx
@@ -11602,12 +11602,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Lato"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -11797,119 +11811,122 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12193,8 +12210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1447"/>
   <sheetViews>
-    <sheetView topLeftCell="A447" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A461" sqref="A461"/>
+    <sheetView topLeftCell="A520" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A537" sqref="A537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -27077,7 +27094,7 @@
     </row>
     <row r="461" spans="1:12" ht="15.5">
       <c r="A461" s="8" t="s">
-        <v>3813</v>
+        <v>1290</v>
       </c>
       <c r="B461" s="8" t="s">
         <v>1307</v>
@@ -59125,10 +59142,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -59157,10 +59174,10 @@
       <c r="E1" s="65" t="s">
         <v>3812</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="68" t="s">
         <v>3847</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="68" t="s">
         <v>3848</v>
       </c>
     </row>
@@ -59168,7 +59185,7 @@
       <c r="A2" s="6" t="s">
         <v>3542</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="67" t="s">
         <v>3815</v>
       </c>
       <c r="F2" s="3">
@@ -59182,7 +59199,7 @@
       <c r="A3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="67" t="s">
         <v>3816</v>
       </c>
       <c r="F3" s="3">
@@ -59196,7 +59213,7 @@
       <c r="A4" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="68" t="s">
+      <c r="E4" s="67" t="s">
         <v>3817</v>
       </c>
       <c r="F4" s="3">
@@ -59210,7 +59227,7 @@
       <c r="A5" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="67" t="s">
         <v>3818</v>
       </c>
       <c r="F5" s="3">
@@ -59224,11 +59241,11 @@
       <c r="A6" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="E6" s="68" t="s">
+      <c r="E6" s="67" t="s">
         <v>3819</v>
       </c>
       <c r="F6" s="3">
-        <v>31.420083299999899</v>
+        <v>-31.420083299999899</v>
       </c>
       <c r="G6" s="3">
         <v>-64.188776099999998</v>
@@ -59238,7 +59255,7 @@
       <c r="A7" s="7" t="s">
         <v>493</v>
       </c>
-      <c r="E7" s="68" t="s">
+      <c r="E7" s="67" t="s">
         <v>3820</v>
       </c>
       <c r="F7" s="3">
@@ -59252,7 +59269,7 @@
       <c r="A8" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="E8" s="68" t="s">
+      <c r="E8" s="67" t="s">
         <v>3821</v>
       </c>
       <c r="F8" s="3">
@@ -59266,7 +59283,7 @@
       <c r="A9" s="6" t="s">
         <v>598</v>
       </c>
-      <c r="E9" s="68" t="s">
+      <c r="E9" s="67" t="s">
         <v>3822</v>
       </c>
       <c r="F9" s="3">
@@ -59280,7 +59297,7 @@
       <c r="A10" s="6" t="s">
         <v>751</v>
       </c>
-      <c r="E10" s="68" t="s">
+      <c r="E10" s="67" t="s">
         <v>3823</v>
       </c>
       <c r="F10" s="3">
@@ -59294,11 +59311,11 @@
       <c r="A11" s="6" t="s">
         <v>921</v>
       </c>
-      <c r="E11" s="68" t="s">
+      <c r="E11" s="67" t="s">
         <v>3824</v>
       </c>
       <c r="F11" s="3">
-        <v>34.603684399999999</v>
+        <v>-34.603684399999999</v>
       </c>
       <c r="G11" s="3">
         <v>-58.381559099999997</v>
@@ -59308,21 +59325,21 @@
       <c r="A12" s="6" t="s">
         <v>971</v>
       </c>
-      <c r="E12" s="68" t="s">
+      <c r="E12" s="70" t="s">
         <v>3825</v>
       </c>
       <c r="F12" s="3">
         <v>-33.047238</v>
       </c>
       <c r="G12" s="3">
-        <v>71.612688499999905</v>
+        <v>-71.612688499999905</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="66" t="s">
         <v>3813</v>
       </c>
-      <c r="E13" s="68" t="s">
+      <c r="E13" s="70" t="s">
         <v>3826</v>
       </c>
       <c r="F13" s="3">
@@ -59336,7 +59353,7 @@
       <c r="A14" s="6" t="s">
         <v>1159</v>
       </c>
-      <c r="E14" s="68" t="s">
+      <c r="E14" s="70" t="s">
         <v>3827</v>
       </c>
       <c r="F14" s="3">
@@ -59350,7 +59367,7 @@
       <c r="A15" s="6" t="s">
         <v>1228</v>
       </c>
-      <c r="E15" s="68" t="s">
+      <c r="E15" s="71" t="s">
         <v>3828</v>
       </c>
       <c r="F15" s="3">
@@ -59361,10 +59378,10 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="69" t="s">
         <v>1290</v>
       </c>
-      <c r="E16" s="68" t="s">
+      <c r="E16" s="70" t="s">
         <v>3829</v>
       </c>
       <c r="F16" s="3">
@@ -59378,7 +59395,7 @@
       <c r="A17" s="7" t="s">
         <v>1371</v>
       </c>
-      <c r="E17" s="68" t="s">
+      <c r="E17" s="70" t="s">
         <v>3830</v>
       </c>
       <c r="F17" s="3">
@@ -59392,7 +59409,7 @@
       <c r="A18" s="6" t="s">
         <v>1397</v>
       </c>
-      <c r="E18" s="67" t="s">
+      <c r="E18" s="72" t="s">
         <v>3814</v>
       </c>
       <c r="F18" s="3">
@@ -59406,7 +59423,7 @@
       <c r="A19" s="6" t="s">
         <v>1434</v>
       </c>
-      <c r="E19" s="68" t="s">
+      <c r="E19" s="70" t="s">
         <v>3815</v>
       </c>
       <c r="F19" s="3">
@@ -59420,7 +59437,7 @@
       <c r="A20" s="7" t="s">
         <v>1821</v>
       </c>
-      <c r="E20" s="68" t="s">
+      <c r="E20" s="70" t="s">
         <v>3831</v>
       </c>
       <c r="F20" s="3">
@@ -59434,7 +59451,7 @@
       <c r="A21" s="7" t="s">
         <v>1840</v>
       </c>
-      <c r="E21" s="68" t="s">
+      <c r="E21" s="70" t="s">
         <v>3832</v>
       </c>
       <c r="F21" s="3">
@@ -59448,7 +59465,7 @@
       <c r="A22" s="7" t="s">
         <v>1853</v>
       </c>
-      <c r="E22" s="68" t="s">
+      <c r="E22" s="70" t="s">
         <v>3833</v>
       </c>
       <c r="F22" s="3">
@@ -59462,7 +59479,7 @@
       <c r="A23" s="7" t="s">
         <v>1864</v>
       </c>
-      <c r="E23" s="68" t="s">
+      <c r="E23" s="70" t="s">
         <v>3834</v>
       </c>
       <c r="F23" s="3">
@@ -59476,7 +59493,7 @@
       <c r="A24" s="7" t="s">
         <v>1873</v>
       </c>
-      <c r="E24" s="68" t="s">
+      <c r="E24" s="70" t="s">
         <v>3835</v>
       </c>
       <c r="F24" s="3">
@@ -59490,7 +59507,7 @@
       <c r="A25" s="7" t="s">
         <v>1879</v>
       </c>
-      <c r="E25" s="68" t="s">
+      <c r="E25" s="70" t="s">
         <v>3836</v>
       </c>
       <c r="F25" s="3">
@@ -59504,11 +59521,11 @@
       <c r="A26" s="6" t="s">
         <v>1887</v>
       </c>
-      <c r="E26" s="68" t="s">
+      <c r="E26" s="70" t="s">
         <v>3837</v>
       </c>
       <c r="F26" s="3">
-        <v>3.3175192999999998</v>
+        <v>-3.3175192999999998</v>
       </c>
       <c r="G26" s="3">
         <v>35.734195300000003</v>
@@ -59518,7 +59535,7 @@
       <c r="A27" s="7" t="s">
         <v>1899</v>
       </c>
-      <c r="E27" s="68" t="s">
+      <c r="E27" s="70" t="s">
         <v>3838</v>
       </c>
       <c r="F27" s="3">
@@ -59532,7 +59549,7 @@
       <c r="A28" s="6" t="s">
         <v>1904</v>
       </c>
-      <c r="E28" s="68" t="s">
+      <c r="E28" s="70" t="s">
         <v>3839</v>
       </c>
       <c r="F28" s="3">
@@ -59546,7 +59563,7 @@
       <c r="A29" s="6" t="s">
         <v>1943</v>
       </c>
-      <c r="E29" s="68" t="s">
+      <c r="E29" s="70" t="s">
         <v>3840</v>
       </c>
       <c r="F29" s="65">
@@ -59560,7 +59577,7 @@
       <c r="A30" s="6" t="s">
         <v>2409</v>
       </c>
-      <c r="E30" s="68" t="s">
+      <c r="E30" s="70" t="s">
         <v>3841</v>
       </c>
       <c r="F30" s="65">
@@ -59574,7 +59591,7 @@
       <c r="A31" s="6" t="s">
         <v>2471</v>
       </c>
-      <c r="E31" s="68" t="s">
+      <c r="E31" s="70" t="s">
         <v>3842</v>
       </c>
       <c r="F31" s="65">
@@ -59588,7 +59605,7 @@
       <c r="A32" s="6" t="s">
         <v>2888</v>
       </c>
-      <c r="E32" s="68" t="s">
+      <c r="E32" s="70" t="s">
         <v>3843</v>
       </c>
       <c r="F32" s="65">
@@ -59602,7 +59619,7 @@
       <c r="A33" s="6" t="s">
         <v>3357</v>
       </c>
-      <c r="E33" s="68" t="s">
+      <c r="E33" s="70" t="s">
         <v>3844</v>
       </c>
       <c r="F33" s="65">
@@ -59616,7 +59633,7 @@
       <c r="A34" s="6" t="s">
         <v>3428</v>
       </c>
-      <c r="E34" s="68" t="s">
+      <c r="E34" s="70" t="s">
         <v>3845</v>
       </c>
       <c r="F34" s="65">
@@ -59630,7 +59647,7 @@
       <c r="A35" s="7" t="s">
         <v>3491</v>
       </c>
-      <c r="E35" s="68" t="s">
+      <c r="E35" s="70" t="s">
         <v>3846</v>
       </c>
       <c r="F35" s="65">
@@ -59639,6 +59656,9 @@
       <c r="G35" s="3">
         <v>-77.036870699999994</v>
       </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="E36" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actually fixed it now woops
</commit_message>
<xml_diff>
--- a/spreadsheets/sponsored_2018.xlsx
+++ b/spreadsheets/sponsored_2018.xlsx
@@ -12207,8 +12207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A447" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A461" sqref="A461"/>
+    <sheetView tabSelected="1" topLeftCell="A519" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A537" sqref="A537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -27091,7 +27091,7 @@
     </row>
     <row r="461" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A461" s="8" t="s">
-        <v>1290</v>
+        <v>3812</v>
       </c>
       <c r="B461" s="8" t="s">
         <v>1306</v>

</xml_diff>